<commit_message>
Added annotation stat plots and excel files
</commit_message>
<xml_diff>
--- a/_lockbox/by_year_sum.xlsx
+++ b/_lockbox/by_year_sum.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t># of annotations</t>
   </si>
@@ -29,12 +29,6 @@
   </si>
   <si>
     <t>2019-12-31</t>
-  </si>
-  <si>
-    <t>2020-12-31</t>
-  </si>
-  <si>
-    <t>2021-12-31</t>
   </si>
   <si>
     <t>2022-12-31</t>
@@ -395,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,22 +432,6 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
         <v>1362</v>
       </c>
     </row>

</xml_diff>